<commit_message>
process power point done
</commit_message>
<xml_diff>
--- a/sprintRetrospective/excel_files/Process.xlsx
+++ b/sprintRetrospective/excel_files/Process.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lessons\documentsLessons\softeng2\project1\sprintRetrospective\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF8FC52-90F8-4A16-9D34-9ECF6FB9B810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458585DF-FFEC-4AF2-B5A0-0426B8CE03C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{37C5AB7B-AEA1-4D1B-9947-DA35975828B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{37C5AB7B-AEA1-4D1B-9947-DA35975828B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
-    <sheet name="tabellaFinale" sheetId="4" r:id="rId2"/>
-    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
-    <sheet name="Foglio2" sheetId="2" r:id="rId4"/>
+    <sheet name="table time with conversion" sheetId="1" r:id="rId1"/>
+    <sheet name="useful data" sheetId="2" r:id="rId2"/>
+    <sheet name="total time" sheetId="3" r:id="rId3"/>
+    <sheet name="useful data table" sheetId="4" r:id="rId4"/>
+    <sheet name="Foglio1" sheetId="7" r:id="rId5"/>
+    <sheet name="time per day" sheetId="5" r:id="rId6"/>
+    <sheet name="charts" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="94">
   <si>
     <t>Stories</t>
   </si>
@@ -229,13 +232,103 @@
   </si>
   <si>
     <t>Actual time converted in hours</t>
+  </si>
+  <si>
+    <t>Total per story</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>E Time</t>
+  </si>
+  <si>
+    <t>Time Spent</t>
+  </si>
+  <si>
+    <t>number of tasks</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>ore</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>task code</t>
+  </si>
+  <si>
+    <t>OQ-13</t>
+  </si>
+  <si>
+    <t>OQ-25</t>
+  </si>
+  <si>
+    <t>OQ-19</t>
+  </si>
+  <si>
+    <t>OQ-14</t>
+  </si>
+  <si>
+    <t>OQ-15</t>
+  </si>
+  <si>
+    <t>OQ-16</t>
+  </si>
+  <si>
+    <t>OQ-17</t>
+  </si>
+  <si>
+    <t>OQ-18</t>
+  </si>
+  <si>
+    <t>OQ-20</t>
+  </si>
+  <si>
+    <t>OQ-21</t>
+  </si>
+  <si>
+    <t>OQ-22</t>
+  </si>
+  <si>
+    <t>OQ-23</t>
+  </si>
+  <si>
+    <t>OQ-24</t>
+  </si>
+  <si>
+    <t>E time</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>total estimation error ratio</t>
+  </si>
+  <si>
+    <t>error ratio</t>
+  </si>
+  <si>
+    <t>avarage hours per task</t>
+  </si>
+  <si>
+    <t>avarage hours per estimated task</t>
+  </si>
+  <si>
+    <t>standard deviation estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard deviation </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +340,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -293,6 +392,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,7 +717,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I20"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f>G3+CONVERT(H3,"mn","hr")</f>
+        <f t="shared" ref="I3:I20" si="0">G3+CONVERT(H3,"mn","hr")</f>
         <v>2</v>
       </c>
       <c r="K3">
@@ -719,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f>G4+CONVERT(H4,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="K4">
@@ -729,7 +835,7 @@
         <v>30</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M20" si="0">K4+CONVERT(L4,"mn","hr")</f>
+        <f t="shared" ref="M4:M20" si="1">K4+CONVERT(L4,"mn","hr")</f>
         <v>11.5</v>
       </c>
     </row>
@@ -750,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <f>G5+CONVERT(H5,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K5">
@@ -760,7 +866,7 @@
         <v>30</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
     </row>
@@ -781,7 +887,7 @@
         <v>15</v>
       </c>
       <c r="I6">
-        <f>G6+CONVERT(H6,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="K6">
@@ -791,7 +897,7 @@
         <v>10</v>
       </c>
       <c r="M6" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -812,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <f>G7+CONVERT(H7,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K7">
@@ -822,7 +928,7 @@
         <v>30</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -834,11 +940,11 @@
         <v>2</v>
       </c>
       <c r="I8">
-        <f>G8+CONVERT(H8,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -859,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <f>G9+CONVERT(H9,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K9">
@@ -869,7 +975,7 @@
         <v>30</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
@@ -890,7 +996,7 @@
         <v>30</v>
       </c>
       <c r="I10">
-        <f>G10+CONVERT(H10,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
       <c r="K10">
@@ -900,7 +1006,7 @@
         <v>30</v>
       </c>
       <c r="M10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
     </row>
@@ -921,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f>G11+CONVERT(H11,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K11">
@@ -931,7 +1037,7 @@
         <v>50</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8333333333333335</v>
       </c>
     </row>
@@ -943,11 +1049,11 @@
         <v>7</v>
       </c>
       <c r="I12">
-        <f>G12+CONVERT(H12,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -968,7 +1074,7 @@
         <v>30</v>
       </c>
       <c r="I13">
-        <f>G13+CONVERT(H13,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="K13">
@@ -978,7 +1084,7 @@
         <v>45</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.75</v>
       </c>
     </row>
@@ -999,7 +1105,7 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <f>G14+CONVERT(H14,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="K14">
@@ -1009,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1021,11 +1127,11 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <f>G15+CONVERT(H15,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1046,7 +1152,7 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <f>G16+CONVERT(H16,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="K16">
@@ -1056,7 +1162,7 @@
         <v>20</v>
       </c>
       <c r="M16" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -1068,11 +1174,11 @@
         <v>12</v>
       </c>
       <c r="I17">
-        <f>G17+CONVERT(H17,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1093,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <f>G18+CONVERT(H18,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K18">
@@ -1103,7 +1209,7 @@
         <v>15</v>
       </c>
       <c r="M18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -1115,11 +1221,11 @@
         <v>15</v>
       </c>
       <c r="I19">
-        <f>G19+CONVERT(H19,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1140,7 +1246,7 @@
         <v>30</v>
       </c>
       <c r="I20">
-        <f>G20+CONVERT(H20,"mn","hr")</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="K20">
@@ -1150,7 +1256,7 @@
         <v>10</v>
       </c>
       <c r="M20" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1666666666666665</v>
       </c>
     </row>
@@ -1161,400 +1267,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA50E4A9-B734-4437-B265-65EF754DB725}">
-  <dimension ref="A1:G20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="82.88671875" customWidth="1"/>
-    <col min="3" max="3" width="67.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" customWidth="1"/>
-    <col min="7" max="7" width="28.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3">
-        <f>Foglio1!I3</f>
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <f>Foglio1!M3</f>
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4">
-        <f>Foglio1!I4</f>
-        <v>8</v>
-      </c>
-      <c r="G4">
-        <f>Foglio1!M4</f>
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5">
-        <f>Foglio1!I5</f>
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <f>Foglio1!M5</f>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <f>Foglio1!I6</f>
-        <v>0.25</v>
-      </c>
-      <c r="G6" s="5">
-        <f>Foglio1!M6</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7">
-        <f>Foglio1!I7</f>
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <f>Foglio1!M7</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9">
-        <f>Foglio1!I9</f>
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <f>Foglio1!M9</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10">
-        <f>Foglio1!I10</f>
-        <v>5.5</v>
-      </c>
-      <c r="G10">
-        <f>Foglio1!M10</f>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11">
-        <f>Foglio1!I11</f>
-        <v>2</v>
-      </c>
-      <c r="G11" s="5">
-        <f>Foglio1!M11</f>
-        <v>1.8333333333333335</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13">
-        <f>Foglio1!I13</f>
-        <v>3.5</v>
-      </c>
-      <c r="G13">
-        <f>Foglio1!M13</f>
-        <v>5.75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14">
-        <f>Foglio1!I14</f>
-        <v>1.5</v>
-      </c>
-      <c r="G14">
-        <f>Foglio1!M14</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16">
-        <f>Foglio1!I16</f>
-        <v>0.5</v>
-      </c>
-      <c r="G16" s="5">
-        <f>Foglio1!M16</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>3</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18">
-        <f>Foglio1!I18</f>
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <f>Foglio1!M18</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20">
-        <f>Foglio1!I20</f>
-        <v>2.5</v>
-      </c>
-      <c r="G20" s="5">
-        <f>Foglio1!M20</f>
-        <v>2.1666666666666665</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC958CDE-D022-4D49-81E2-9A3F7A7F23FD}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.77734375" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <f>SUM(Foglio1!A2:A19)</f>
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <f>SUM(Foglio1!I3:I20)</f>
-        <v>35.75</v>
-      </c>
-      <c r="C3" s="5">
-        <f>SUM(Foglio1!M3:M20)</f>
-        <v>41.25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95A5DC6-B31B-4EFB-99AC-0C3F4FAB067C}">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D12" sqref="D12:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,11 +1472,11 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <f>Foglio2!G3/5</f>
+        <f>'table time with conversion'!I3/5</f>
         <v>0.4</v>
       </c>
       <c r="D12">
-        <f>Foglio2!K3/5</f>
+        <f>'table time with conversion'!M3/5</f>
         <v>0.45</v>
       </c>
     </row>
@@ -1768,11 +1485,11 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <f>Foglio2!G4/5</f>
-        <v>1.2</v>
+        <f>'table time with conversion'!I4/5</f>
+        <v>1.6</v>
       </c>
       <c r="D13">
-        <f>Foglio2!K4/5</f>
+        <f>'table time with conversion'!M4/5</f>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -1781,11 +1498,11 @@
         <v>18</v>
       </c>
       <c r="C14">
-        <f>Foglio2!G5/5</f>
+        <f>'table time with conversion'!I5/5</f>
         <v>0.8</v>
       </c>
       <c r="D14">
-        <f>Foglio2!K5/5</f>
+        <f>'table time with conversion'!M5/5</f>
         <v>0.9</v>
       </c>
     </row>
@@ -1794,11 +1511,11 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <f>Foglio2!G6/5</f>
+        <f>'table time with conversion'!I6/5</f>
         <v>0.05</v>
       </c>
-      <c r="D15" s="5">
-        <f>Foglio2!K6/5</f>
+      <c r="D15">
+        <f>'table time with conversion'!M6/5</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -1807,15 +1524,955 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <f>Foglio2!G7/5</f>
+        <f>'table time with conversion'!I7/5</f>
         <v>0.2</v>
       </c>
       <c r="D16">
-        <f>Foglio2!K7/5</f>
+        <f>'table time with conversion'!M7/5</f>
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC958CDE-D022-4D49-81E2-9A3F7A7F23FD}">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" customWidth="1"/>
+    <col min="11" max="11" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>SUM('table time with conversion'!A2:A19)</f>
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f>SUM('table time with conversion'!I3:I20)</f>
+        <v>35.75</v>
+      </c>
+      <c r="C3" s="5">
+        <f>SUM('table time with conversion'!M3:M20)</f>
+        <v>41.25</v>
+      </c>
+      <c r="G3" s="5">
+        <f>B3/C3</f>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="J3">
+        <f>B3/13</f>
+        <v>2.75</v>
+      </c>
+      <c r="K3" s="5">
+        <f>C3/13</f>
+        <v>3.1730769230769229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f>SUM('table time with conversion'!I9:I11,'table time with conversion'!I3,'table time with conversion'!I6) + 'useful data'!C13</f>
+        <v>14.35</v>
+      </c>
+      <c r="C9" s="5">
+        <f>SUM('useful data table'!G9:G11,'useful data table'!G3,'useful data table'!G6) + 'useful data'!D13</f>
+        <v>16.55</v>
+      </c>
+      <c r="D9">
+        <f>COUNTA('useful data table'!G9:G11,'useful data table'!G3,'useful data table'!G6)</f>
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5">
+        <f>B9/C9</f>
+        <v>0.86706948640483383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>SUM('table time with conversion'!I13:I14,'table time with conversion'!I7,'table time with conversion'!I5)+ 'useful data'!C13</f>
+        <v>11.6</v>
+      </c>
+      <c r="C10">
+        <f>SUM('useful data table'!G13:G14,'useful data table'!G5,'useful data table'!G7) + 'useful data'!D13</f>
+        <v>14.05</v>
+      </c>
+      <c r="D10">
+        <f>COUNTA('useful data table'!G13:G14,'useful data table'!G5,'useful data table'!G7)</f>
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" ref="F10:F13" si="0">B10/C10</f>
+        <v>0.82562277580071164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <f>SUM('table time with conversion'!I16)+ 'useful data'!C13</f>
+        <v>2.1</v>
+      </c>
+      <c r="C11" s="5">
+        <f>SUM('useful data table'!G16)+ 'useful data'!D13</f>
+        <v>2.6333333333333333</v>
+      </c>
+      <c r="D11">
+        <f>COUNTA('useful data table'!G16)</f>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.79746835443037978</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <f>SUM('table time with conversion'!I18)+ 'useful data'!C13</f>
+        <v>3.6</v>
+      </c>
+      <c r="C12">
+        <f>SUM('useful data table'!G18)+ 'useful data'!D13</f>
+        <v>3.55</v>
+      </c>
+      <c r="D12">
+        <f>COUNTA('useful data table'!G18)</f>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0140845070422535</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <f>SUM('table time with conversion'!I20)+ 'useful data'!C13</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C13" s="5">
+        <f>SUM('useful data table'!G20)+ 'useful data'!D13</f>
+        <v>4.4666666666666668</v>
+      </c>
+      <c r="D13">
+        <f>COUNTA('useful data table'!G20)</f>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.9179104477611939</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J18" s="5">
+        <f>STDEV('table time with conversion'!I3:I7,'table time with conversion'!I9:I11,'table time with conversion'!I13:I14,'table time with conversion'!I16,'table time with conversion'!I18,'table time with conversion'!I20)</f>
+        <v>2.1408720964441881</v>
+      </c>
+      <c r="K18" s="5">
+        <f>STDEV('table time with conversion'!M3:M7,'table time with conversion'!M9:M11,'table time with conversion'!M13:M14,'table time with conversion'!M16,'table time with conversion'!M18,'table time with conversion'!M20)</f>
+        <v>3.2306155420642026</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA50E4A9-B734-4437-B265-65EF754DB725}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="82.88671875" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" customWidth="1"/>
+    <col min="7" max="7" width="28.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3">
+        <f>'table time with conversion'!I3</f>
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f>'table time with conversion'!M3</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <f>'table time with conversion'!I4</f>
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <f>'table time with conversion'!M4</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <f>'table time with conversion'!I5</f>
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <f>'table time with conversion'!M5</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <f>'table time with conversion'!I6</f>
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="5">
+        <f>'table time with conversion'!M6</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <f>'table time with conversion'!I7</f>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f>'table time with conversion'!M7</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <f>'table time with conversion'!I9</f>
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <f>'table time with conversion'!M9</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="C10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <f>'table time with conversion'!I10</f>
+        <v>5.5</v>
+      </c>
+      <c r="G10">
+        <f>'table time with conversion'!M10</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="C11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <f>'table time with conversion'!I11</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="5">
+        <f>'table time with conversion'!M11</f>
+        <v>1.8333333333333335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13">
+        <f>'table time with conversion'!I13</f>
+        <v>3.5</v>
+      </c>
+      <c r="G13">
+        <f>'table time with conversion'!M13</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14">
+        <f>'table time with conversion'!I14</f>
+        <v>1.5</v>
+      </c>
+      <c r="G14">
+        <f>'table time with conversion'!M14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16">
+        <f>'table time with conversion'!I16</f>
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="5">
+        <f>'table time with conversion'!M16</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18">
+        <f>'table time with conversion'!I18</f>
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <f>'table time with conversion'!M18</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20">
+        <f>'table time with conversion'!I20</f>
+        <v>2.5</v>
+      </c>
+      <c r="G20" s="5">
+        <f>'table time with conversion'!M20</f>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD46363-1123-4C18-B770-F6851009B863}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A2EB66-1B22-4FC8-93C4-AC1872D3A118}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L17:L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F86247E-35C9-4DCD-A0D6-0056444BD794}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="71.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>0+1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2">
+        <f>'table time with conversion'!I3</f>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f>'table time with conversion'!M3</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3">
+        <f>'table time with conversion'!I4</f>
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <f>'table time with conversion'!M4</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A14" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <f>'table time with conversion'!I5</f>
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <f>'table time with conversion'!M5</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <f>'table time with conversion'!I6</f>
+        <v>0.25</v>
+      </c>
+      <c r="E5">
+        <f>'table time with conversion'!M6</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6">
+        <f>'table time with conversion'!I7</f>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>'table time with conversion'!M7</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7">
+        <f>'table time with conversion'!I9</f>
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <f>'table time with conversion'!M9</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8">
+        <f>'table time with conversion'!I10</f>
+        <v>5.5</v>
+      </c>
+      <c r="E8">
+        <f>'table time with conversion'!M10</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9">
+        <f>'table time with conversion'!I11</f>
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f>'table time with conversion'!M11</f>
+        <v>1.8333333333333335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10">
+        <f>'table time with conversion'!I13</f>
+        <v>3.5</v>
+      </c>
+      <c r="E10">
+        <f>'table time with conversion'!M13</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11">
+        <f>'table time with conversion'!I14</f>
+        <v>1.5</v>
+      </c>
+      <c r="E11">
+        <f>'table time with conversion'!M14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>A11+1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12">
+        <f>'table time with conversion'!I16</f>
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <f>'table time with conversion'!M16</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13">
+        <f>'table time with conversion'!I18</f>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>'table time with conversion'!M18</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14">
+        <f>'table time with conversion'!I20</f>
+        <v>2.5</v>
+      </c>
+      <c r="E14">
+        <f>'table time with conversion'!M20</f>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>